<commit_message>
Python scripts to use vw and perform cross validation.
</commit_message>
<xml_diff>
--- a/code/Errors on single feature predictions.xlsx
+++ b/code/Errors on single feature predictions.xlsx
@@ -105,12 +105,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,8 +155,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,11 +411,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="182831008"/>
-        <c:axId val="184086768"/>
+        <c:axId val="110585184"/>
+        <c:axId val="44464864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182831008"/>
+        <c:axId val="110585184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,7 +514,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184086768"/>
+        <c:crossAx val="44464864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -487,7 +522,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184086768"/>
+        <c:axId val="44464864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -538,7 +573,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182831008"/>
+        <c:crossAx val="110585184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1431,7 +1466,7 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,37 +1487,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="O1" t="s">

</xml_diff>